<commit_message>
fix event memory when assign company
</commit_message>
<xml_diff>
--- a/Source/PQT.Web/Content/SampleFiles/company_resources_sample.xlsx
+++ b/Source/PQT.Web/Content/SampleFiles/company_resources_sample.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20730"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{0E422979-E30B-4FC0-BCC3-B99DF9A3BFD4}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9417CF74-72E7-4ABC-AEDC-CC2B881390F2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="36">
   <si>
     <t>Country</t>
   </si>
@@ -120,6 +120,9 @@
   </si>
   <si>
     <t>BudgetMonth</t>
+  </si>
+  <si>
+    <t>DirectLine</t>
   </si>
 </sst>
 </file>
@@ -614,10 +617,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{918DBEA7-D683-4612-9DF9-78DDF48D7CBF}">
-  <dimension ref="A1:M5"/>
+  <dimension ref="A1:N5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -627,13 +630,14 @@
     <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="36.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="32" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.42578125" customWidth="1"/>
+    <col min="8" max="10" width="32" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -653,28 +657,31 @@
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="2" t="s">
         <v>8</v>
@@ -691,19 +698,20 @@
       <c r="F2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="5"/>
+      <c r="H2" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="H2" s="5"/>
       <c r="I2" s="5"/>
-      <c r="J2" s="7" t="s">
+      <c r="J2" s="5"/>
+      <c r="K2" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="M2">
+      <c r="N2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
       <c r="B3" s="2" t="s">
         <v>8</v>
@@ -718,16 +726,17 @@
       <c r="F3" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="G3" s="5"/>
+      <c r="H3" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="H3" s="5"/>
       <c r="I3" s="5"/>
-      <c r="J3" s="6" t="s">
+      <c r="J3" s="5"/>
+      <c r="K3" s="6" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
       <c r="B4" s="2" t="s">
         <v>8</v>
@@ -742,19 +751,20 @@
       <c r="F4" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="G4" s="5"/>
+      <c r="H4" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="H4" s="5"/>
       <c r="I4" s="5"/>
-      <c r="J4" s="6" t="s">
+      <c r="J4" s="5"/>
+      <c r="K4" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="M4">
+      <c r="N4">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
       <c r="B5" s="2" t="s">
         <v>8</v>
@@ -769,12 +779,13 @@
       <c r="F5" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="G5" s="5"/>
+      <c r="H5" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="H5" s="5"/>
       <c r="I5" s="5"/>
-      <c r="J5" s="6" t="s">
+      <c r="J5" s="5"/>
+      <c r="K5" s="6" t="s">
         <v>26</v>
       </c>
     </row>

</xml_diff>